<commit_message>
added hyphy results to spreadsheet
</commit_message>
<xml_diff>
--- a/doc/distances.xlsx
+++ b/doc/distances.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="36600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="distances.tsv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>n/a</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Solyc09g005080.1</t>
   </si>
   <si>
-    <t>Solyc09g010080.2</t>
-  </si>
-  <si>
     <t>Solyc09g010090.2</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Solyc10g083290.1</t>
   </si>
   <si>
-    <t>Solyc11g071430.1</t>
-  </si>
-  <si>
     <t>Gene ID</t>
   </si>
   <si>
@@ -94,6 +88,66 @@
   </si>
   <si>
     <t>S. lycopersicum (U0015716-1891)</t>
+  </si>
+  <si>
+    <t>0.040829846**</t>
+  </si>
+  <si>
+    <t>0.079610741**</t>
+  </si>
+  <si>
+    <t>0.126323981**</t>
+  </si>
+  <si>
+    <t>0.229670853**</t>
+  </si>
+  <si>
+    <t>0.019536514**</t>
+  </si>
+  <si>
+    <t>0.043066278**</t>
+  </si>
+  <si>
+    <t>0.066494491**</t>
+  </si>
+  <si>
+    <t>0.058671364**</t>
+  </si>
+  <si>
+    <t>0.200437053**</t>
+  </si>
+  <si>
+    <t>0.046789914**</t>
+  </si>
+  <si>
+    <t>0.064766918**</t>
+  </si>
+  <si>
+    <t>Solyc09g010080.2**</t>
+  </si>
+  <si>
+    <t>0.030330532**</t>
+  </si>
+  <si>
+    <t>0.014732076**</t>
+  </si>
+  <si>
+    <t>0.053833837**</t>
+  </si>
+  <si>
+    <t>0.025578612**</t>
+  </si>
+  <si>
+    <t>0.016771483**</t>
+  </si>
+  <si>
+    <t>0.104439962**</t>
+  </si>
+  <si>
+    <t>Solyc11g071430.1**</t>
+  </si>
+  <si>
+    <t>0.002932947**</t>
   </si>
 </sst>
 </file>
@@ -103,7 +157,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +169,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,10 +201,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
@@ -478,64 +540,64 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="B1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="8" width="17.33203125" style="1"/>
+    <col min="2" max="8" width="19.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>4.0829846000000003E-2</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
-        <v>7.9610740999999999E-2</v>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E2" s="1">
         <v>5.1348786E-2</v>
       </c>
-      <c r="F2" s="1">
-        <v>0.126323981</v>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G2" s="1">
         <v>7.8162000000000001E-4</v>
       </c>
-      <c r="H2" s="1">
-        <v>0.22967085300000001</v>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -591,7 +653,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -632,8 +694,8 @@
       <c r="E6" s="1">
         <v>1.0343197E-2</v>
       </c>
-      <c r="F6" s="1">
-        <v>1.9536514000000001E-2</v>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="G6" s="2">
         <v>2.4999999999999999E-8</v>
@@ -669,29 +731,29 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>4.3066278E-2</v>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C8" s="1">
         <v>4.8442365000000001E-2</v>
       </c>
-      <c r="D8" s="1">
-        <v>6.6494491000000003E-2</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5.8671363999999997E-2</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.200437053</v>
-      </c>
-      <c r="G8" s="1">
-        <v>4.6789914000000002E-2</v>
-      </c>
-      <c r="H8" s="1">
-        <v>6.4766918000000007E-2</v>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -774,7 +836,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1">
         <v>2.3848378E-2</v>
@@ -788,19 +850,19 @@
       <c r="E12" s="1">
         <v>7.536587E-3</v>
       </c>
-      <c r="F12" s="1">
-        <v>3.0330532E-2</v>
+      <c r="F12" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="G12" s="2">
         <v>0</v>
       </c>
-      <c r="H12" s="1">
-        <v>1.4732076E-2</v>
+      <c r="H12" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>8.0706370000000003E-3</v>
@@ -817,16 +879,16 @@
       <c r="F13" s="2">
         <v>7.1999999999999996E-8</v>
       </c>
-      <c r="G13" s="1">
-        <v>5.3833837000000002E-2</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2.5578612000000001E-2</v>
+      <c r="G13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>7.4052120000000004E-3</v>
@@ -852,7 +914,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>0</v>
@@ -878,7 +940,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>1.3346454000000001E-2</v>
@@ -895,22 +957,22 @@
       <c r="F16" s="1">
         <v>1.1785350000000001E-3</v>
       </c>
-      <c r="G16" s="1">
-        <v>1.6771483E-2</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0.104439962</v>
+      <c r="G16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="1">
-        <v>2.932947E-3</v>
+      <c r="C17" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="D17" s="1">
         <v>3.5455769999999998E-3</v>

</xml_diff>